<commit_message>
Long time,I haven`t study my investigation.
</commit_message>
<xml_diff>
--- a/入れ子式交差検証結果.xlsx
+++ b/入れ子式交差検証結果.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icech\Desktop\share\Lab\2018_07_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DACAC3-013C-4FB4-8AD7-A53844DDF899}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520A540C-BD36-4245-8057-B9133000F662}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9120" xr2:uid="{B8A84C3E-AD93-44C4-BBD2-F4F46764C3B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="5664" xr2:uid="{B8A84C3E-AD93-44C4-BBD2-F4F46764C3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>末尾4語　ファイル数28対28</t>
     <rPh sb="0" eb="2">
@@ -134,6 +134,47 @@
     </rPh>
     <rPh sb="3" eb="4">
       <t>レツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自民党</t>
+    <rPh sb="0" eb="3">
+      <t>ジミントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>民主党</t>
+    <rPh sb="0" eb="3">
+      <t>ミンシュトウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>総数</t>
+    <rPh sb="0" eb="2">
+      <t>ソウスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再現率</t>
+    <rPh sb="0" eb="2">
+      <t>サイゲン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>適合率</t>
+    <rPh sb="0" eb="2">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>リツ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -142,6 +183,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -401,13 +445,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -451,233 +644,64 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1028,18 +1052,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56393A6B-A211-4CD1-A7AB-8F75F898E40F}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="3" width="17.296875" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="17.296875" customWidth="1"/>
+    <col min="1" max="1" width="33.09765625" customWidth="1"/>
+    <col min="2" max="2" width="9.69921875" customWidth="1"/>
+    <col min="3" max="3" width="9.19921875" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="7.3984375" customWidth="1"/>
     <col min="6" max="6" width="8.796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1271,16 +1296,95 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
+    <row r="26" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="27" spans="2:9" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="B28" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="20">
+        <v>57.1</v>
+      </c>
+      <c r="D28" s="21">
+        <v>80</v>
+      </c>
+      <c r="E28" s="22">
+        <v>28</v>
+      </c>
+      <c r="F28" s="22">
+        <v>16</v>
+      </c>
+      <c r="G28" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="B29" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="16">
+        <v>85.7</v>
+      </c>
+      <c r="D29" s="15">
+        <v>66.7</v>
+      </c>
+      <c r="E29" s="15">
+        <v>28</v>
+      </c>
+      <c r="F29" s="15">
+        <v>4</v>
+      </c>
+      <c r="G29" s="28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="22.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="29">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D30" s="30">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="E30" s="30">
+        <v>56</v>
+      </c>
+      <c r="F30" s="30">
+        <v>20</v>
+      </c>
+      <c r="G30" s="31">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="top10" dxfId="6" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D5">
-    <cfRule type="top10" dxfId="4" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E5">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>

</xml_diff>